<commit_message>
commiting code to master
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testData.xlsx
+++ b/src/test/resources/testdata/testData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D77E14DC-51FB-41E3-ACA2-93085807887F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6EB62C43-79D3-45EE-A2E4-C415D37031E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="15405" windowHeight="11820" xr2:uid="{845CB9C4-2866-4311-9FF1-5E8FED9AC6BA}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="15555" windowHeight="11820" xr2:uid="{845CB9C4-2866-4311-9FF1-5E8FED9AC6BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="1" r:id="rId1"/>
@@ -124,28 +124,28 @@
     <t>""</t>
   </si>
   <si>
-    <t>ibu18@gmail.com</t>
-  </si>
-  <si>
-    <t>deepti.kharbanda18@gmail.com</t>
-  </si>
-  <si>
-    <t>kartika.varma18@gmail.com</t>
-  </si>
-  <si>
-    <t>kavita.kharbanda18@gmail.com</t>
-  </si>
-  <si>
-    <t>1000000019</t>
-  </si>
-  <si>
-    <t>1000000020</t>
-  </si>
-  <si>
-    <t>1000000021</t>
-  </si>
-  <si>
-    <t>1000000022</t>
+    <t>kavita.kharbanda22@gmail.com</t>
+  </si>
+  <si>
+    <t>ibu22@gmail.com</t>
+  </si>
+  <si>
+    <t>deepti.kharbanda22@gmail.com</t>
+  </si>
+  <si>
+    <t>1000000031</t>
+  </si>
+  <si>
+    <t>1000000032</t>
+  </si>
+  <si>
+    <t>1000000033</t>
+  </si>
+  <si>
+    <t>1000000034</t>
+  </si>
+  <si>
+    <t>kartika.varma22@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -512,7 +512,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,10 +552,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -572,10 +572,10 @@
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -592,10 +592,10 @@
         <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -612,10 +612,10 @@
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
adding the selenoid code in the fw
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testData.xlsx
+++ b/src/test/resources/testdata/testData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9369D0FF-D214-4C9F-AF5C-447D53747DCD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{16304FEE-8FF6-4CF1-B7F3-96AE81FE7645}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="15645" windowHeight="11820" xr2:uid="{845CB9C4-2866-4311-9FF1-5E8FED9AC6BA}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="15735" windowHeight="11820" xr2:uid="{845CB9C4-2866-4311-9FF1-5E8FED9AC6BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="1" r:id="rId1"/>
@@ -124,28 +124,28 @@
     <t>""</t>
   </si>
   <si>
-    <t>ibu25@gmail.com</t>
-  </si>
-  <si>
-    <t>deepti.kharbanda25@gmail.com</t>
-  </si>
-  <si>
-    <t>kartika.varma25@gmail.com</t>
-  </si>
-  <si>
-    <t>kavita.kharbanda25@gmail.com</t>
-  </si>
-  <si>
-    <t>1000000042</t>
-  </si>
-  <si>
-    <t>1000000043</t>
-  </si>
-  <si>
-    <t>1000000044</t>
-  </si>
-  <si>
-    <t>1000000045</t>
+    <t>ibu28@gmail.com</t>
+  </si>
+  <si>
+    <t>deepti.kharbanda28@gmail.com</t>
+  </si>
+  <si>
+    <t>kartika.varma28@gmail.com</t>
+  </si>
+  <si>
+    <t>kavita.kharbanda28@gmail.com</t>
+  </si>
+  <si>
+    <t>1000000054</t>
+  </si>
+  <si>
+    <t>1000000055</t>
+  </si>
+  <si>
+    <t>1000000056</t>
+  </si>
+  <si>
+    <t>1000000057</t>
   </si>
 </sst>
 </file>
@@ -512,7 +512,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>